<commit_message>
New restriction sites added
</commit_message>
<xml_diff>
--- a/6res_2.xlsx
+++ b/6res_2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>UID</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Deionised water</t>
-  </si>
-  <si>
-    <t>A2</t>
   </si>
 </sst>
 </file>
@@ -393,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -454,32 +451,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>2875</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>